<commit_message>
Copy Files From Source Repo (2025-05-27 04:01)
</commit_message>
<xml_diff>
--- a/ResourceFiles/Contoso Chai Tea market trends.xlsx
+++ b/ResourceFiles/Contoso Chai Tea market trends.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/tfrink_microsoft_com/Documents/Documents/BUSS/Learn courses/MS-4004 - V2 Mar 2025/Source docs/LP2-Empower your workforce with M365 use cases/M4-Marketing use case/track changes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Projects\LeX\FY25\ILT\MSU121821_ILT_May\MS-4004_GitHub\10_DTP\de-DE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A92FE4-727D-4E00-8BEF-6A1CBB54089B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId3"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -279,22 +279,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="m/d/yyyy"/>
-  </numFmts>
-  <fonts count="5">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -345,74 +336,25 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="4">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <u val="none"/>
-        <strike val="0"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <color theme="1"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" shrinkToFit="0" readingOrder="0"/>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="177" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <border>
@@ -430,147 +372,29 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
         <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.7999799847602844"/>
-          <bgColor theme="4" tint="0.7999799847602844"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" shrinkToFit="0" readingOrder="0"/>
       <border>
-        <vertical style="thin">
-          <color theme="0"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="0"/>
-        </horizontal>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thick">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thick">
-          <color theme="0"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.5999900102615356"/>
-          <bgColor theme="4" tint="0.5999900102615356"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -583,15 +407,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F13" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="2" headerRowBorderDxfId="3">
-  <autoFilter ref="A1:F13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F13" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A1:F13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Monat" dataDxfId="1"/>
-    <tableColumn id="2" name="Chai-Verkäufe insgesamt (Einheiten)"/>
-    <tableColumn id="3" name="Verkäufe von Artisanal Chai  (Einheiten)"/>
-    <tableColumn id="4" name="Vorgefertigter Chai-Umsatz (Einheiten)"/>
-    <tableColumn id="5" name="Social-Media-Interaktion (Ansichten)"/>
-    <tableColumn id="6" name="Onlinesuchen nach Chai"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Monat" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Chai-Verkäufe insgesamt (Einheiten)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Verkäufe von Artisanal Chai  (Einheiten)"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Vorgefertigter Chai-Umsatz (Einheiten)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Social-Media-Interaktion (Ansichten)"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Onlinesuchen nach Chai"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -883,24 +707,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection pane="topLeft" activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.285714285714286" customWidth="1"/>
-    <col min="2" max="2" width="16.571428571428573" customWidth="1"/>
-    <col min="3" max="3" width="17.857142857142858" customWidth="1"/>
-    <col min="4" max="4" width="19.571428571428573" customWidth="1"/>
-    <col min="5" max="5" width="24.857142857142858" customWidth="1"/>
-    <col min="6" max="6" width="14.571428571428571" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8">
+    <row r="1" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -920,12 +744,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <f t="shared" si="0" ref="B2:B13">SUM(C2+D2)</f>
+        <f t="shared" ref="B2:B13" si="0">SUM(C2+D2)</f>
         <v>659</v>
       </c>
       <c r="C2">
@@ -941,7 +765,7 @@
         <v>2663</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -962,7 +786,7 @@
         <v>2546</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -983,7 +807,7 @@
         <v>2371</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1004,7 +828,7 @@
         <v>2996</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1025,7 +849,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1046,7 +870,7 @@
         <v>5016</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1067,7 +891,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1088,7 +912,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1109,7 +933,7 @@
         <v>2784</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1130,7 +954,7 @@
         <v>2663</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1151,7 +975,7 @@
         <v>2546</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1174,7 +998,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts>
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>

</xml_diff>